<commit_message>
Portal Check Added and Asana Updates
</commit_message>
<xml_diff>
--- a/Data/Asana.xlsx
+++ b/Data/Asana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcsweeney\Desktop\UiDemo Testing\RPA Vendor Dispute Bot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3802012C-8044-49E1-AAAE-74703E652317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8D5C79-1952-4AC0-9C67-A16F17360E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1215" windowWidth="21600" windowHeight="11175" xr2:uid="{C86CC469-5493-4F8D-ABB6-DF992D8F219B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8074BBC3-4930-422A-897F-104497A3607B}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="2" r:id="rId1"/>
@@ -482,14 +482,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04973530-8B52-45A9-AB5E-514A60362331}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8039207-BBAB-426A-98B7-CAFBF027D685}">
   <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,12 +572,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE8BA98-DB04-4EA7-B097-A360DC03E7DD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EBDDCC-4238-4E9A-97EE-6B77F29A5B67}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>